<commit_message>
added new cases + update temple dataset
</commit_message>
<xml_diff>
--- a/data/list_hindu_temples_in_pak/20230408_list_hindu_temples_pakistan.xlsx
+++ b/data/list_hindu_temples_in_pak/20230408_list_hindu_temples_pakistan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/list_hindu_temples_in_pak/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB3FD26-ADC6-EB4B-BEA1-4837275A7408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670BCCC8-CFE9-8D45-BA64-29BB068E2E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{F972FD0D-5727-664D-8ADB-B0BAD774D1DF}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="list_hindu_temples_in_pak" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list_hindu_temples_in_pak!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list_hindu_temples_in_pak!$A$1:$P$344</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="610">
   <si>
     <t>serial_number</t>
   </si>
@@ -1812,6 +1812,63 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1623594706104987648</t>
+  </si>
+  <si>
+    <t>Ancient Jain Temple</t>
+  </si>
+  <si>
+    <t>Ancient Ruined Jain Temple, Road, Nagarparkar, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Old Jain Temple</t>
+  </si>
+  <si>
+    <t>9PVJ+4WP, Unnamed Road, Bhodisar, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Bhodisar</t>
+  </si>
+  <si>
+    <t>Bhodisar Temple 1</t>
+  </si>
+  <si>
+    <t>Pooni Jain Temple (Bhodisar Temple 3)</t>
+  </si>
+  <si>
+    <t>9PWJ+2G8, Nagarparkar, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Ashoka Temple</t>
+  </si>
+  <si>
+    <t>9PVJ+4JR, Bhodisar, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Sadourus Jain Temple</t>
+  </si>
+  <si>
+    <t>CQQV+CRM, Sadorus, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Godiji Jain Derasar</t>
+  </si>
+  <si>
+    <t>JJQ9+735, Islam Kot-Nagar Parkar Rd, Antri, Sindh, Guri, Tharparkar, Sindh, Pakistan</t>
+  </si>
+  <si>
+    <t>Dado Mosani Shah</t>
+  </si>
+  <si>
+    <t>Keenlothur</t>
+  </si>
+  <si>
+    <t>8PGF+G6, Keenlothur, Tharparkar, Sindh, Pakistan</t>
   </si>
 </sst>
 </file>
@@ -2178,9 +2235,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4996F06-64E2-9640-BC5E-872CBC50CF4C}">
-  <dimension ref="A1:P344"/>
+  <dimension ref="A1:Q351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B316" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L351" sqref="L351"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2188,7 +2250,7 @@
     <col min="8" max="8" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2237,8 +2299,11 @@
       <c r="P1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2273,7 +2338,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2308,7 +2373,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2331,7 +2396,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2351,7 +2416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2371,7 +2436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2400,7 +2465,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2420,7 +2485,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2448,8 +2513,20 @@
       <c r="L9" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>590</v>
+      </c>
+      <c r="N9" t="s">
+        <v>590</v>
+      </c>
+      <c r="O9" t="s">
+        <v>586</v>
+      </c>
+      <c r="P9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2469,7 +2546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2498,7 +2575,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2518,7 +2595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2541,7 +2618,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2561,7 +2638,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2590,7 +2667,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4917,7 +4994,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4939,8 +5016,26 @@
       <c r="H113" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J113" t="s">
+        <v>435</v>
+      </c>
+      <c r="M113" t="b">
+        <v>1</v>
+      </c>
+      <c r="N113" t="b">
+        <v>1</v>
+      </c>
+      <c r="O113" t="b">
+        <v>0</v>
+      </c>
+      <c r="P113" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4963,7 +5058,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4986,7 +5081,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5009,7 +5104,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5032,7 +5127,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5064,7 +5159,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5087,7 +5182,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5110,7 +5205,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5133,7 +5228,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5159,7 +5254,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5191,7 +5286,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5214,7 +5309,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5237,7 +5332,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5260,7 +5355,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5292,7 +5387,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9334,7 +9429,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>288</v>
       </c>
@@ -9357,7 +9452,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>289</v>
       </c>
@@ -9380,7 +9475,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>290</v>
       </c>
@@ -9403,7 +9498,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>291</v>
       </c>
@@ -9426,7 +9521,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>292</v>
       </c>
@@ -9449,7 +9544,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>293</v>
       </c>
@@ -9463,19 +9558,34 @@
         <v>356</v>
       </c>
       <c r="F294" s="2">
-        <v>24.389522500000002</v>
+        <v>24.286096157593601</v>
       </c>
       <c r="G294" s="2">
-        <v>71.036405099999996</v>
+        <v>70.780502965023004</v>
       </c>
       <c r="H294" t="s">
-        <v>361</v>
+        <v>593</v>
       </c>
       <c r="J294" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L294" t="s">
+        <v>449</v>
+      </c>
+      <c r="M294" t="s">
+        <v>590</v>
+      </c>
+      <c r="N294" t="s">
+        <v>590</v>
+      </c>
+      <c r="O294" t="s">
+        <v>586</v>
+      </c>
+      <c r="P294" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>294</v>
       </c>
@@ -9507,7 +9617,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>295</v>
       </c>
@@ -9530,7 +9640,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>296</v>
       </c>
@@ -9553,7 +9663,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>297</v>
       </c>
@@ -9576,7 +9686,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>298</v>
       </c>
@@ -9599,7 +9709,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>299</v>
       </c>
@@ -9631,7 +9741,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>300</v>
       </c>
@@ -9654,7 +9764,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>301</v>
       </c>
@@ -9686,7 +9796,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>302</v>
       </c>
@@ -9718,7 +9828,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>303</v>
       </c>
@@ -10582,7 +10692,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>336</v>
       </c>
@@ -10611,7 +10721,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>337</v>
       </c>
@@ -10643,7 +10753,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>338</v>
       </c>
@@ -10666,7 +10776,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>339</v>
       </c>
@@ -10689,7 +10799,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>340</v>
       </c>
@@ -10721,7 +10831,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>341</v>
       </c>
@@ -10741,7 +10851,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>342</v>
       </c>
@@ -10761,7 +10871,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>343</v>
       </c>
@@ -10784,8 +10894,304 @@
         <v>426</v>
       </c>
     </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>344</v>
+      </c>
+      <c r="B345" t="s">
+        <v>173</v>
+      </c>
+      <c r="C345" t="s">
+        <v>349</v>
+      </c>
+      <c r="D345" t="s">
+        <v>597</v>
+      </c>
+      <c r="E345" t="s">
+        <v>594</v>
+      </c>
+      <c r="F345" s="2">
+        <v>24.355175540046499</v>
+      </c>
+      <c r="G345">
+        <v>70.753503809273894</v>
+      </c>
+      <c r="H345" t="s">
+        <v>595</v>
+      </c>
+      <c r="J345" t="s">
+        <v>360</v>
+      </c>
+      <c r="L345" t="s">
+        <v>449</v>
+      </c>
+      <c r="M345" t="s">
+        <v>590</v>
+      </c>
+      <c r="N345" t="s">
+        <v>590</v>
+      </c>
+      <c r="O345" t="s">
+        <v>586</v>
+      </c>
+      <c r="P345" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>345</v>
+      </c>
+      <c r="B346" t="s">
+        <v>173</v>
+      </c>
+      <c r="C346" t="s">
+        <v>349</v>
+      </c>
+      <c r="D346" t="s">
+        <v>597</v>
+      </c>
+      <c r="E346" t="s">
+        <v>596</v>
+      </c>
+      <c r="F346" s="2">
+        <v>24.3929669403025</v>
+      </c>
+      <c r="G346">
+        <v>70.732635040299797</v>
+      </c>
+      <c r="H346" t="s">
+        <v>598</v>
+      </c>
+      <c r="J346" t="s">
+        <v>360</v>
+      </c>
+      <c r="L346" t="s">
+        <v>449</v>
+      </c>
+      <c r="M346" t="s">
+        <v>590</v>
+      </c>
+      <c r="N346" t="s">
+        <v>590</v>
+      </c>
+      <c r="O346" t="s">
+        <v>586</v>
+      </c>
+      <c r="P346" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <v>346</v>
+      </c>
+      <c r="B347" t="s">
+        <v>173</v>
+      </c>
+      <c r="C347" t="s">
+        <v>349</v>
+      </c>
+      <c r="D347" t="s">
+        <v>597</v>
+      </c>
+      <c r="E347" t="s">
+        <v>600</v>
+      </c>
+      <c r="F347">
+        <v>24.395164924541799</v>
+      </c>
+      <c r="G347">
+        <v>70.731935564577199</v>
+      </c>
+      <c r="H347" t="s">
+        <v>599</v>
+      </c>
+      <c r="J347" t="s">
+        <v>360</v>
+      </c>
+      <c r="L347" t="s">
+        <v>449</v>
+      </c>
+      <c r="M347" t="s">
+        <v>590</v>
+      </c>
+      <c r="N347" t="s">
+        <v>590</v>
+      </c>
+      <c r="O347" t="s">
+        <v>586</v>
+      </c>
+      <c r="P347" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="348" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <v>347</v>
+      </c>
+      <c r="B348" t="s">
+        <v>173</v>
+      </c>
+      <c r="C348" t="s">
+        <v>349</v>
+      </c>
+      <c r="D348" t="s">
+        <v>597</v>
+      </c>
+      <c r="E348" t="s">
+        <v>602</v>
+      </c>
+      <c r="F348" s="2">
+        <v>24.392970724747101</v>
+      </c>
+      <c r="G348">
+        <v>70.731497564985304</v>
+      </c>
+      <c r="H348" t="s">
+        <v>601</v>
+      </c>
+      <c r="J348" t="s">
+        <v>360</v>
+      </c>
+      <c r="M348" t="s">
+        <v>590</v>
+      </c>
+      <c r="N348" t="s">
+        <v>590</v>
+      </c>
+      <c r="O348" t="s">
+        <v>586</v>
+      </c>
+      <c r="P348" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <v>348</v>
+      </c>
+      <c r="B349" t="s">
+        <v>173</v>
+      </c>
+      <c r="C349" t="s">
+        <v>349</v>
+      </c>
+      <c r="D349" t="s">
+        <v>597</v>
+      </c>
+      <c r="E349" t="s">
+        <v>604</v>
+      </c>
+      <c r="F349">
+        <v>24.438613848833601</v>
+      </c>
+      <c r="G349">
+        <v>70.794550825716001</v>
+      </c>
+      <c r="H349" t="s">
+        <v>603</v>
+      </c>
+      <c r="J349" t="s">
+        <v>360</v>
+      </c>
+      <c r="M349" t="s">
+        <v>590</v>
+      </c>
+      <c r="N349" t="s">
+        <v>586</v>
+      </c>
+      <c r="O349" t="s">
+        <v>586</v>
+      </c>
+      <c r="P349" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="350" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <v>349</v>
+      </c>
+      <c r="B350" t="s">
+        <v>173</v>
+      </c>
+      <c r="C350" t="s">
+        <v>349</v>
+      </c>
+      <c r="D350" t="s">
+        <v>374</v>
+      </c>
+      <c r="E350" t="s">
+        <v>606</v>
+      </c>
+      <c r="F350">
+        <v>24.645466319712899</v>
+      </c>
+      <c r="G350">
+        <v>70.648275374994299</v>
+      </c>
+      <c r="H350" t="s">
+        <v>605</v>
+      </c>
+      <c r="J350" t="s">
+        <v>360</v>
+      </c>
+      <c r="M350" t="s">
+        <v>590</v>
+      </c>
+      <c r="N350" t="s">
+        <v>590</v>
+      </c>
+      <c r="O350" t="s">
+        <v>586</v>
+      </c>
+      <c r="P350" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <v>350</v>
+      </c>
+      <c r="B351" t="s">
+        <v>173</v>
+      </c>
+      <c r="C351" t="s">
+        <v>349</v>
+      </c>
+      <c r="D351" t="s">
+        <v>608</v>
+      </c>
+      <c r="E351" t="s">
+        <v>609</v>
+      </c>
+      <c r="F351">
+        <v>24.326362338719299</v>
+      </c>
+      <c r="G351">
+        <v>69.723175184720404</v>
+      </c>
+      <c r="H351" t="s">
+        <v>607</v>
+      </c>
+      <c r="J351" t="s">
+        <v>360</v>
+      </c>
+      <c r="M351" t="s">
+        <v>590</v>
+      </c>
+      <c r="N351" t="s">
+        <v>590</v>
+      </c>
+      <c r="O351" t="s">
+        <v>586</v>
+      </c>
+      <c r="P351" t="s">
+        <v>586</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P1" xr:uid="{E4996F06-64E2-9640-BC5E-872CBC50CF4C}"/>
+  <autoFilter ref="A1:P344" xr:uid="{E4996F06-64E2-9640-BC5E-872CBC50CF4C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>